<commit_message>
added functions to the sql fragment generator
</commit_message>
<xml_diff>
--- a/artifacts/query_gen_schemas/query_gen_schemas.xlsx
+++ b/artifacts/query_gen_schemas/query_gen_schemas.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\research_projects\speakql2_to_sql\artifacts\query_gen_schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A863C952-AE48-40FF-8D35-51947B98718C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A24FA-62C7-43A3-896E-62F2BE78F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9370" yWindow="2230" windowWidth="19200" windowHeight="11260"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="177">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -548,12 +558,15 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>IS_NUMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1390,11 +1403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G239"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B226" sqref="B226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1408,7 +1421,7 @@
     <col min="7" max="7" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1430,8 +1443,11 @@
       <c r="G1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1447,8 +1463,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1461,8 +1480,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1475,8 +1497,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1492,8 +1517,11 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1515,8 +1543,11 @@
       <c r="G6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1529,8 +1560,11 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1543,8 +1577,11 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1594,11 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1574,8 +1614,11 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1597,8 +1640,11 @@
       <c r="G11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1620,8 +1666,11 @@
       <c r="G12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1643,8 +1692,11 @@
       <c r="G13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1657,8 +1709,11 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1671,8 +1726,11 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1685,8 +1743,11 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1699,8 +1760,11 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1713,8 +1777,11 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1730,8 +1797,11 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1744,8 +1814,11 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1761,8 +1834,11 @@
       <c r="E21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1784,8 +1860,11 @@
       <c r="G22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1798,8 +1877,11 @@
       <c r="D23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1812,8 +1894,11 @@
       <c r="D24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1826,8 +1911,11 @@
       <c r="D25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1840,8 +1928,11 @@
       <c r="D26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1854,8 +1945,11 @@
       <c r="D27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1877,8 +1971,11 @@
       <c r="G28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1891,8 +1988,11 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1905,8 +2005,11 @@
       <c r="D30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1919,8 +2022,11 @@
       <c r="D31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1933,8 +2039,11 @@
       <c r="D32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -1948,8 +2057,11 @@
         <v>6</v>
       </c>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1965,8 +2077,11 @@
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -1988,8 +2103,11 @@
       <c r="G35" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2003,8 +2121,11 @@
         <v>51</v>
       </c>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2026,8 +2147,11 @@
       <c r="G37" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -2041,8 +2165,11 @@
         <v>53</v>
       </c>
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2058,8 +2185,11 @@
       <c r="E39" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2073,8 +2203,11 @@
         <v>53</v>
       </c>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2088,8 +2221,11 @@
         <v>16</v>
       </c>
       <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2103,8 +2239,11 @@
         <v>6</v>
       </c>
       <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2120,8 +2259,11 @@
       <c r="E43" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2135,8 +2277,11 @@
         <v>51</v>
       </c>
       <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -2150,8 +2295,11 @@
         <v>16</v>
       </c>
       <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -2167,8 +2315,11 @@
       <c r="E46" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2182,8 +2333,11 @@
         <v>53</v>
       </c>
       <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2197,8 +2351,11 @@
         <v>63</v>
       </c>
       <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2212,8 +2369,11 @@
         <v>65</v>
       </c>
       <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2227,8 +2387,11 @@
         <v>65</v>
       </c>
       <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -2242,8 +2405,11 @@
         <v>53</v>
       </c>
       <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2257,8 +2423,11 @@
         <v>53</v>
       </c>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2272,8 +2441,11 @@
         <v>48</v>
       </c>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2287,8 +2459,11 @@
         <v>65</v>
       </c>
       <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2302,8 +2477,11 @@
         <v>53</v>
       </c>
       <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -2317,8 +2495,11 @@
         <v>53</v>
       </c>
       <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -2332,8 +2513,11 @@
         <v>16</v>
       </c>
       <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2347,8 +2531,11 @@
         <v>53</v>
       </c>
       <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2362,8 +2549,11 @@
         <v>65</v>
       </c>
       <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2379,8 +2569,11 @@
       <c r="E60" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -2394,8 +2587,11 @@
         <v>63</v>
       </c>
       <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -2411,8 +2607,11 @@
       <c r="E62" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2426,8 +2625,11 @@
         <v>65</v>
       </c>
       <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -2443,8 +2645,11 @@
       <c r="E64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2457,8 +2662,11 @@
       <c r="D65" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2474,8 +2682,11 @@
       <c r="E66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2488,8 +2699,11 @@
       <c r="D67" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -2502,8 +2716,11 @@
       <c r="D68" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2516,8 +2733,11 @@
       <c r="D69" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -2530,8 +2750,11 @@
       <c r="D70" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2544,8 +2767,11 @@
       <c r="D71" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2558,8 +2784,11 @@
       <c r="D72" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -2572,8 +2801,11 @@
       <c r="D73" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2589,8 +2821,11 @@
       <c r="E74" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -2612,8 +2847,11 @@
       <c r="G75" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -2626,8 +2864,11 @@
       <c r="D76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2640,8 +2881,11 @@
       <c r="D77" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -2657,8 +2901,11 @@
       <c r="E78" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2671,8 +2918,11 @@
       <c r="D79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2685,8 +2935,11 @@
       <c r="D80" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2702,8 +2955,11 @@
       <c r="E81" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2716,8 +2972,11 @@
       <c r="D82" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -2730,8 +2989,11 @@
       <c r="D83" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -2744,8 +3006,11 @@
       <c r="D84" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -2761,8 +3026,11 @@
       <c r="E85" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -2784,8 +3052,11 @@
       <c r="G86" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -2798,8 +3069,11 @@
       <c r="D87" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -2821,8 +3095,11 @@
       <c r="G88" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>80</v>
       </c>
@@ -2835,8 +3112,11 @@
       <c r="D89" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>80</v>
       </c>
@@ -2852,8 +3132,11 @@
       <c r="E90" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -2866,8 +3149,11 @@
       <c r="D91" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -2880,8 +3166,11 @@
       <c r="D92" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -2894,8 +3183,11 @@
       <c r="D93" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>80</v>
       </c>
@@ -2911,8 +3203,11 @@
       <c r="E94" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>80</v>
       </c>
@@ -2925,8 +3220,11 @@
       <c r="D95" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>80</v>
       </c>
@@ -2939,8 +3237,11 @@
       <c r="D96" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -2956,8 +3257,11 @@
       <c r="E97" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -2970,8 +3274,11 @@
       <c r="D98" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>80</v>
       </c>
@@ -2984,8 +3291,11 @@
       <c r="D99" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>80</v>
       </c>
@@ -2998,8 +3308,11 @@
       <c r="D100" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>80</v>
       </c>
@@ -3012,8 +3325,11 @@
       <c r="D101" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>80</v>
       </c>
@@ -3026,8 +3342,11 @@
       <c r="D102" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>80</v>
       </c>
@@ -3040,8 +3359,11 @@
       <c r="D103" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>80</v>
       </c>
@@ -3054,8 +3376,11 @@
       <c r="D104" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>80</v>
       </c>
@@ -3068,8 +3393,11 @@
       <c r="D105" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>80</v>
       </c>
@@ -3082,8 +3410,11 @@
       <c r="D106" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>80</v>
       </c>
@@ -3096,8 +3427,11 @@
       <c r="D107" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>80</v>
       </c>
@@ -3110,8 +3444,11 @@
       <c r="D108" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -3124,8 +3461,11 @@
       <c r="D109" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>80</v>
       </c>
@@ -3138,8 +3478,11 @@
       <c r="D110" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>80</v>
       </c>
@@ -3152,8 +3495,11 @@
       <c r="D111" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>80</v>
       </c>
@@ -3175,8 +3521,11 @@
       <c r="G112" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -3189,8 +3538,11 @@
       <c r="D113" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>80</v>
       </c>
@@ -3206,8 +3558,11 @@
       <c r="E114" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>80</v>
       </c>
@@ -3220,8 +3575,11 @@
       <c r="D115" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>80</v>
       </c>
@@ -3234,8 +3592,11 @@
       <c r="D116" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>80</v>
       </c>
@@ -3251,8 +3612,11 @@
       <c r="E117" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -3265,8 +3629,11 @@
       <c r="D118" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>80</v>
       </c>
@@ -3288,8 +3655,11 @@
       <c r="G119" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>80</v>
       </c>
@@ -3302,8 +3672,11 @@
       <c r="D120" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>80</v>
       </c>
@@ -3316,8 +3689,11 @@
       <c r="D121" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>80</v>
       </c>
@@ -3330,8 +3706,11 @@
       <c r="D122" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>80</v>
       </c>
@@ -3344,8 +3723,11 @@
       <c r="D123" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>80</v>
       </c>
@@ -3358,8 +3740,11 @@
       <c r="D124" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>80</v>
       </c>
@@ -3372,8 +3757,11 @@
       <c r="D125" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>80</v>
       </c>
@@ -3386,8 +3774,11 @@
       <c r="D126" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -3400,8 +3791,11 @@
       <c r="D127" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>80</v>
       </c>
@@ -3414,8 +3808,11 @@
       <c r="D128" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>80</v>
       </c>
@@ -3428,8 +3825,11 @@
       <c r="D129" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>80</v>
       </c>
@@ -3445,8 +3845,11 @@
       <c r="E130" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>80</v>
       </c>
@@ -3468,8 +3871,11 @@
       <c r="G131" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>80</v>
       </c>
@@ -3482,8 +3888,11 @@
       <c r="D132" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>80</v>
       </c>
@@ -3496,8 +3905,11 @@
       <c r="D133" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>80</v>
       </c>
@@ -3519,8 +3931,11 @@
       <c r="G134" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>80</v>
       </c>
@@ -3533,8 +3948,11 @@
       <c r="D135" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>80</v>
       </c>
@@ -3547,8 +3965,11 @@
       <c r="D136" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -3561,8 +3982,11 @@
       <c r="D137" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>80</v>
       </c>
@@ -3575,8 +3999,11 @@
       <c r="D138" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>80</v>
       </c>
@@ -3589,8 +4016,11 @@
       <c r="D139" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>80</v>
       </c>
@@ -3603,8 +4033,11 @@
       <c r="D140" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>80</v>
       </c>
@@ -3620,8 +4053,11 @@
       <c r="E141" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>80</v>
       </c>
@@ -3637,8 +4073,11 @@
       <c r="E142" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>80</v>
       </c>
@@ -3654,8 +4093,11 @@
       <c r="E143" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>80</v>
       </c>
@@ -3668,8 +4110,11 @@
       <c r="D144" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>80</v>
       </c>
@@ -3685,8 +4130,11 @@
       <c r="E145" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -3702,8 +4150,11 @@
       <c r="E146" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>80</v>
       </c>
@@ -3716,8 +4167,11 @@
       <c r="D147" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>80</v>
       </c>
@@ -3730,8 +4184,11 @@
       <c r="D148" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -3744,8 +4201,11 @@
       <c r="D149" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>80</v>
       </c>
@@ -3758,8 +4218,11 @@
       <c r="D150" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>80</v>
       </c>
@@ -3772,8 +4235,11 @@
       <c r="D151" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>80</v>
       </c>
@@ -3786,8 +4252,11 @@
       <c r="D152" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>80</v>
       </c>
@@ -3800,8 +4269,11 @@
       <c r="D153" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>80</v>
       </c>
@@ -3814,8 +4286,11 @@
       <c r="D154" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>80</v>
       </c>
@@ -3828,8 +4303,11 @@
       <c r="D155" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>80</v>
       </c>
@@ -3842,8 +4320,11 @@
       <c r="D156" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>80</v>
       </c>
@@ -3859,8 +4340,11 @@
       <c r="E157" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>80</v>
       </c>
@@ -3876,8 +4360,11 @@
       <c r="E158" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>80</v>
       </c>
@@ -3899,8 +4386,11 @@
       <c r="G159" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>80</v>
       </c>
@@ -3916,8 +4406,11 @@
       <c r="E160" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>80</v>
       </c>
@@ -3930,8 +4423,11 @@
       <c r="D161" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>80</v>
       </c>
@@ -3953,8 +4449,11 @@
       <c r="G162" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>80</v>
       </c>
@@ -3970,8 +4469,11 @@
       <c r="E163" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>80</v>
       </c>
@@ -3984,8 +4486,11 @@
       <c r="D164" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>80</v>
       </c>
@@ -3998,8 +4503,11 @@
       <c r="D165" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>80</v>
       </c>
@@ -4012,8 +4520,11 @@
       <c r="D166" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>80</v>
       </c>
@@ -4026,8 +4537,11 @@
       <c r="D167" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>80</v>
       </c>
@@ -4040,8 +4554,11 @@
       <c r="D168" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>80</v>
       </c>
@@ -4054,8 +4571,11 @@
       <c r="D169" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>80</v>
       </c>
@@ -4068,8 +4588,11 @@
       <c r="D170" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -4082,8 +4605,11 @@
       <c r="D171" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>80</v>
       </c>
@@ -4096,8 +4622,11 @@
       <c r="D172" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>80</v>
       </c>
@@ -4110,8 +4639,11 @@
       <c r="D173" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>80</v>
       </c>
@@ -4124,8 +4656,11 @@
       <c r="D174" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>80</v>
       </c>
@@ -4141,8 +4676,11 @@
       <c r="E175" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>80</v>
       </c>
@@ -4155,8 +4693,11 @@
       <c r="D176" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>80</v>
       </c>
@@ -4169,8 +4710,11 @@
       <c r="D177" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>80</v>
       </c>
@@ -4186,8 +4730,11 @@
       <c r="E178" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H178" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>80</v>
       </c>
@@ -4209,8 +4756,11 @@
       <c r="G179" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>80</v>
       </c>
@@ -4232,8 +4782,11 @@
       <c r="G180" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H180" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>80</v>
       </c>
@@ -4255,8 +4808,11 @@
       <c r="G181" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H181" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>80</v>
       </c>
@@ -4278,8 +4834,11 @@
       <c r="G182" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>80</v>
       </c>
@@ -4292,8 +4851,11 @@
       <c r="D183" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>80</v>
       </c>
@@ -4309,8 +4871,11 @@
       <c r="E184" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>80</v>
       </c>
@@ -4326,8 +4891,11 @@
       <c r="E185" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H185" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>80</v>
       </c>
@@ -4340,8 +4908,11 @@
       <c r="D186" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>80</v>
       </c>
@@ -4363,8 +4934,11 @@
       <c r="G187" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H187" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>80</v>
       </c>
@@ -4377,8 +4951,11 @@
       <c r="D188" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>80</v>
       </c>
@@ -4391,8 +4968,11 @@
       <c r="D189" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -4405,8 +4985,11 @@
       <c r="D190" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>80</v>
       </c>
@@ -4419,8 +5002,11 @@
       <c r="D191" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>80</v>
       </c>
@@ -4433,8 +5019,11 @@
       <c r="D192" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>80</v>
       </c>
@@ -4447,8 +5036,11 @@
       <c r="D193" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H193" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>80</v>
       </c>
@@ -4470,8 +5062,11 @@
       <c r="G194" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H194" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>80</v>
       </c>
@@ -4484,8 +5079,11 @@
       <c r="D195" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>80</v>
       </c>
@@ -4498,8 +5096,11 @@
       <c r="D196" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>80</v>
       </c>
@@ -4512,8 +5113,11 @@
       <c r="D197" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>80</v>
       </c>
@@ -4526,8 +5130,11 @@
       <c r="D198" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>80</v>
       </c>
@@ -4540,8 +5147,11 @@
       <c r="D199" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>80</v>
       </c>
@@ -4554,8 +5164,11 @@
       <c r="D200" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>80</v>
       </c>
@@ -4571,8 +5184,11 @@
       <c r="E201" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>80</v>
       </c>
@@ -4594,8 +5210,11 @@
       <c r="G202" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H202" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>80</v>
       </c>
@@ -4608,8 +5227,11 @@
       <c r="D203" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>80</v>
       </c>
@@ -4622,8 +5244,11 @@
       <c r="D204" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>80</v>
       </c>
@@ -4636,8 +5261,11 @@
       <c r="D205" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>80</v>
       </c>
@@ -4650,8 +5278,11 @@
       <c r="D206" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>80</v>
       </c>
@@ -4664,8 +5295,11 @@
       <c r="D207" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>80</v>
       </c>
@@ -4678,8 +5312,11 @@
       <c r="D208" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>80</v>
       </c>
@@ -4692,8 +5329,11 @@
       <c r="D209" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>80</v>
       </c>
@@ -4706,8 +5346,11 @@
       <c r="D210" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H210" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>80</v>
       </c>
@@ -4720,8 +5363,11 @@
       <c r="D211" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>80</v>
       </c>
@@ -4743,8 +5389,11 @@
       <c r="G212" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H212" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>80</v>
       </c>
@@ -4757,8 +5406,11 @@
       <c r="D213" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>80</v>
       </c>
@@ -4780,8 +5432,11 @@
       <c r="G214" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>80</v>
       </c>
@@ -4797,8 +5452,11 @@
       <c r="E215" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>158</v>
       </c>
@@ -4814,8 +5472,11 @@
       <c r="E216" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>158</v>
       </c>
@@ -4828,8 +5489,11 @@
       <c r="D217" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H217" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>158</v>
       </c>
@@ -4845,8 +5509,11 @@
       <c r="E218" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H218" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>158</v>
       </c>
@@ -4868,8 +5535,11 @@
       <c r="G219" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>158</v>
       </c>
@@ -4882,8 +5552,11 @@
       <c r="D220" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>158</v>
       </c>
@@ -4896,8 +5569,11 @@
       <c r="D221" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>158</v>
       </c>
@@ -4919,8 +5595,11 @@
       <c r="G222" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>158</v>
       </c>
@@ -4936,8 +5615,11 @@
       <c r="E223" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H223" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>158</v>
       </c>
@@ -4950,8 +5632,11 @@
       <c r="D224" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H224" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>158</v>
       </c>
@@ -4964,8 +5649,11 @@
       <c r="D225" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>158</v>
       </c>
@@ -4981,8 +5669,11 @@
       <c r="E226" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H226" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>158</v>
       </c>
@@ -4995,8 +5686,11 @@
       <c r="D227" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H227" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>158</v>
       </c>
@@ -5009,8 +5703,11 @@
       <c r="D228" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H228" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>158</v>
       </c>
@@ -5023,8 +5720,11 @@
       <c r="D229" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>158</v>
       </c>
@@ -5037,8 +5737,11 @@
       <c r="D230" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H230" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>158</v>
       </c>
@@ -5051,8 +5754,11 @@
       <c r="D231" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>158</v>
       </c>
@@ -5074,8 +5780,11 @@
       <c r="G232" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H232" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>158</v>
       </c>
@@ -5088,8 +5797,11 @@
       <c r="D233" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H233" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -5102,8 +5814,11 @@
       <c r="D234" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H234" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>158</v>
       </c>
@@ -5116,8 +5831,11 @@
       <c r="D235" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H235" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>158</v>
       </c>
@@ -5139,8 +5857,11 @@
       <c r="G236" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H236" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>158</v>
       </c>
@@ -5153,8 +5874,11 @@
       <c r="D237" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H237" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>158</v>
       </c>
@@ -5167,8 +5891,11 @@
       <c r="D238" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H238" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>158</v>
       </c>
@@ -5180,6 +5907,9 @@
       </c>
       <c r="D239" t="s">
         <v>37</v>
+      </c>
+      <c r="H239" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fragment generator to randomize order of select from and where expressions
</commit_message>
<xml_diff>
--- a/artifacts/query_gen_schemas/query_gen_schemas.xlsx
+++ b/artifacts/query_gen_schemas/query_gen_schemas.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\research_projects\speakql2_to_sql\artifacts\query_gen_schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A24FA-62C7-43A3-896E-62F2BE78F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5305A844-0CE2-4E51-BFF2-5085D08EFF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">column_names!$A$1:$H$239</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1404,10 +1407,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H240" sqref="H240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,7 +1451,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1501,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1521,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1598,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1615,10 +1619,10 @@
         <v>7</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1670,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1713,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1730,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1801,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1818,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1881,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1975,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2009,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2061,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2078,10 +2082,10 @@
         <v>7</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2104,10 +2108,10 @@
         <v>49</v>
       </c>
       <c r="H35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2125,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2151,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -2169,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2186,10 +2190,10 @@
         <v>7</v>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2225,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2243,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2260,10 +2264,10 @@
         <v>7</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2337,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -2409,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2463,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2481,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -2517,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2553,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2573,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -2591,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -2646,10 +2650,10 @@
         <v>7</v>
       </c>
       <c r="H64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2666,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2686,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2703,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -2717,10 +2721,10 @@
         <v>48</v>
       </c>
       <c r="H68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -2754,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2788,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -2805,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2822,10 +2826,10 @@
         <v>7</v>
       </c>
       <c r="H74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -2848,10 +2852,10 @@
         <v>47</v>
       </c>
       <c r="H75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2885,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2939,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2956,10 +2960,10 @@
         <v>7</v>
       </c>
       <c r="H81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2976,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -2993,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -3010,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -3027,10 +3031,10 @@
         <v>7</v>
       </c>
       <c r="H85" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -3053,10 +3057,10 @@
         <v>49</v>
       </c>
       <c r="H86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -3099,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>80</v>
       </c>
@@ -3116,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>80</v>
       </c>
@@ -3133,10 +3137,10 @@
         <v>7</v>
       </c>
       <c r="H90" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -3187,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>80</v>
       </c>
@@ -3204,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="H94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>80</v>
       </c>
@@ -3241,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -3261,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>80</v>
       </c>
@@ -3329,7 +3333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>80</v>
       </c>
@@ -3346,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>80</v>
       </c>
@@ -3397,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>80</v>
       </c>
@@ -3414,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>80</v>
       </c>
@@ -3448,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -3499,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>80</v>
       </c>
@@ -3522,10 +3526,10 @@
         <v>90</v>
       </c>
       <c r="H112" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>80</v>
       </c>
@@ -3559,10 +3563,10 @@
         <v>7</v>
       </c>
       <c r="H114" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>80</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>80</v>
       </c>
@@ -3596,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>80</v>
       </c>
@@ -3616,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -3633,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>80</v>
       </c>
@@ -3656,10 +3660,10 @@
         <v>105</v>
       </c>
       <c r="H119" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>80</v>
       </c>
@@ -3676,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>80</v>
       </c>
@@ -3693,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>80</v>
       </c>
@@ -3710,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>80</v>
       </c>
@@ -3724,10 +3728,10 @@
         <v>48</v>
       </c>
       <c r="H123" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>80</v>
       </c>
@@ -3744,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>80</v>
       </c>
@@ -3761,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>80</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -3792,10 +3796,10 @@
         <v>98</v>
       </c>
       <c r="H127" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>80</v>
       </c>
@@ -3812,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>80</v>
       </c>
@@ -3829,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>80</v>
       </c>
@@ -3846,10 +3850,10 @@
         <v>7</v>
       </c>
       <c r="H130" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>80</v>
       </c>
@@ -3872,10 +3876,10 @@
         <v>113</v>
       </c>
       <c r="H131" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>80</v>
       </c>
@@ -3909,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>80</v>
       </c>
@@ -3932,10 +3936,10 @@
         <v>113</v>
       </c>
       <c r="H134" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>80</v>
       </c>
@@ -3952,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>80</v>
       </c>
@@ -3986,7 +3990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>80</v>
       </c>
@@ -4003,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>80</v>
       </c>
@@ -4020,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>80</v>
       </c>
@@ -4037,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>80</v>
       </c>
@@ -4057,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>80</v>
       </c>
@@ -4074,10 +4078,10 @@
         <v>7</v>
       </c>
       <c r="H142" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>80</v>
       </c>
@@ -4094,10 +4098,10 @@
         <v>7</v>
       </c>
       <c r="H143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>80</v>
       </c>
@@ -4114,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>80</v>
       </c>
@@ -4131,10 +4135,10 @@
         <v>7</v>
       </c>
       <c r="H145" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -4151,10 +4155,10 @@
         <v>7</v>
       </c>
       <c r="H146" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>80</v>
       </c>
@@ -4171,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>80</v>
       </c>
@@ -4188,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -4205,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>80</v>
       </c>
@@ -4222,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>80</v>
       </c>
@@ -4236,7 +4240,7 @@
         <v>48</v>
       </c>
       <c r="H151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
@@ -4256,7 +4260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>80</v>
       </c>
@@ -4273,7 +4277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>80</v>
       </c>
@@ -4290,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>80</v>
       </c>
@@ -4307,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>80</v>
       </c>
@@ -4324,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>80</v>
       </c>
@@ -4341,10 +4345,10 @@
         <v>7</v>
       </c>
       <c r="H157" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>80</v>
       </c>
@@ -4364,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>80</v>
       </c>
@@ -4387,10 +4391,10 @@
         <v>112</v>
       </c>
       <c r="H159" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>80</v>
       </c>
@@ -4410,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>80</v>
       </c>
@@ -4427,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>80</v>
       </c>
@@ -4450,10 +4454,10 @@
         <v>105</v>
       </c>
       <c r="H162" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>80</v>
       </c>
@@ -4470,10 +4474,10 @@
         <v>7</v>
       </c>
       <c r="H163" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>80</v>
       </c>
@@ -4490,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>80</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>80</v>
       </c>
@@ -4524,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>80</v>
       </c>
@@ -4541,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>80</v>
       </c>
@@ -4558,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>80</v>
       </c>
@@ -4572,7 +4576,7 @@
         <v>48</v>
       </c>
       <c r="H169" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -4592,7 +4596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -4609,7 +4613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>80</v>
       </c>
@@ -4626,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>80</v>
       </c>
@@ -4643,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>80</v>
       </c>
@@ -4660,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>80</v>
       </c>
@@ -4677,10 +4681,10 @@
         <v>12</v>
       </c>
       <c r="H175" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>80</v>
       </c>
@@ -4697,7 +4701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>80</v>
       </c>
@@ -4714,7 +4718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>80</v>
       </c>
@@ -4731,10 +4735,10 @@
         <v>7</v>
       </c>
       <c r="H178" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>80</v>
       </c>
@@ -4757,10 +4761,10 @@
         <v>139</v>
       </c>
       <c r="H179" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>80</v>
       </c>
@@ -4783,10 +4787,10 @@
         <v>140</v>
       </c>
       <c r="H180" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>80</v>
       </c>
@@ -4809,10 +4813,10 @@
         <v>103</v>
       </c>
       <c r="H181" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>80</v>
       </c>
@@ -4838,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>80</v>
       </c>
@@ -4855,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>80</v>
       </c>
@@ -4875,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>80</v>
       </c>
@@ -4892,10 +4896,10 @@
         <v>7</v>
       </c>
       <c r="H185" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>80</v>
       </c>
@@ -4912,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>80</v>
       </c>
@@ -4935,10 +4939,10 @@
         <v>140</v>
       </c>
       <c r="H187" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>80</v>
       </c>
@@ -4955,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>80</v>
       </c>
@@ -4972,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -4989,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>80</v>
       </c>
@@ -5006,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>80</v>
       </c>
@@ -5040,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>80</v>
       </c>
@@ -5063,10 +5067,10 @@
         <v>90</v>
       </c>
       <c r="H194" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>80</v>
       </c>
@@ -5083,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>80</v>
       </c>
@@ -5100,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>80</v>
       </c>
@@ -5117,7 +5121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>80</v>
       </c>
@@ -5134,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>80</v>
       </c>
@@ -5151,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>80</v>
       </c>
@@ -5168,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>80</v>
       </c>
@@ -5185,10 +5189,10 @@
         <v>7</v>
       </c>
       <c r="H201" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>80</v>
       </c>
@@ -5211,10 +5215,10 @@
         <v>105</v>
       </c>
       <c r="H202" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>80</v>
       </c>
@@ -5231,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>80</v>
       </c>
@@ -5248,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>80</v>
       </c>
@@ -5265,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>80</v>
       </c>
@@ -5282,7 +5286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>80</v>
       </c>
@@ -5296,10 +5300,10 @@
         <v>98</v>
       </c>
       <c r="H207" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>80</v>
       </c>
@@ -5316,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>80</v>
       </c>
@@ -5333,7 +5337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>80</v>
       </c>
@@ -5347,10 +5351,10 @@
         <v>98</v>
       </c>
       <c r="H210" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>80</v>
       </c>
@@ -5367,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>80</v>
       </c>
@@ -5390,10 +5394,10 @@
         <v>90</v>
       </c>
       <c r="H212" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>80</v>
       </c>
@@ -5410,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>80</v>
       </c>
@@ -5433,10 +5437,10 @@
         <v>140</v>
       </c>
       <c r="H214" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>80</v>
       </c>
@@ -5453,10 +5457,10 @@
         <v>7</v>
       </c>
       <c r="H215" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>158</v>
       </c>
@@ -5476,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>158</v>
       </c>
@@ -5510,10 +5514,10 @@
         <v>7</v>
       </c>
       <c r="H218" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>158</v>
       </c>
@@ -5539,7 +5543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>158</v>
       </c>
@@ -5556,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>158</v>
       </c>
@@ -5573,7 +5577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>158</v>
       </c>
@@ -5616,10 +5620,10 @@
         <v>7</v>
       </c>
       <c r="H223" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>158</v>
       </c>
@@ -5636,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>158</v>
       </c>
@@ -5670,10 +5674,10 @@
         <v>7</v>
       </c>
       <c r="H226" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>158</v>
       </c>
@@ -5690,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>158</v>
       </c>
@@ -5707,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>158</v>
       </c>
@@ -5724,7 +5728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>158</v>
       </c>
@@ -5741,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>158</v>
       </c>
@@ -5781,7 +5785,7 @@
         <v>162</v>
       </c>
       <c r="H232" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.35">
@@ -5801,7 +5805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -5818,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>158</v>
       </c>
@@ -5858,10 +5862,10 @@
         <v>162</v>
       </c>
       <c r="H236" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>158</v>
       </c>
@@ -5878,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>158</v>
       </c>
@@ -5895,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>158</v>
       </c>
@@ -5913,6 +5917,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H239" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added multi relation joins to query generator
</commit_message>
<xml_diff>
--- a/artifacts/query_gen_schemas/query_gen_schemas.xlsx
+++ b/artifacts/query_gen_schemas/query_gen_schemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\research_projects\speakql2_to_sql\artifacts\query_gen_schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5305A844-0CE2-4E51-BFF2-5085D08EFF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB6BF7-2CCD-48ED-BCEF-F07102F8BD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="690" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="1" r:id="rId1"/>
@@ -1411,7 +1411,7 @@
   <dimension ref="A1:H239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H240" sqref="H240"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>80</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>80</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>80</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>80</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>80</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>80</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>80</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>80</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>80</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>80</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>80</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>80</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>80</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>80</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>80</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>80</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>80</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>80</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>80</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>80</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>80</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>80</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>80</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>80</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>80</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>80</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>80</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>158</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>158</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>158</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>158</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>158</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>158</v>
       </c>
@@ -5918,10 +5918,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H239" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated speakql query generator to use distinct values from university database
</commit_message>
<xml_diff>
--- a/artifacts/query_gen_schemas/query_gen_schemas.xlsx
+++ b/artifacts/query_gen_schemas/query_gen_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\research_projects\speakql2_to_sql\artifacts\query_gen_schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB6BF7-2CCD-48ED-BCEF-F07102F8BD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC2EA25-AE77-42EC-B083-9803A13F392C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="690" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="1" r:id="rId1"/>
@@ -1407,11 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1451,7 +1450,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1602,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1700,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2247,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>78</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -2521,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2557,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -2653,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2707,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -2724,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2792,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2855,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -2909,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>80</v>
       </c>
@@ -3120,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>80</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -3157,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -3174,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>80</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>80</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>80</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>80</v>
       </c>
@@ -3299,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>80</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>80</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>80</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>80</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>80</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>80</v>
       </c>
@@ -3401,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>80</v>
       </c>
@@ -3418,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>80</v>
       </c>
@@ -3435,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>80</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>80</v>
       </c>
@@ -3486,7 +3485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>80</v>
       </c>
@@ -3529,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -3546,7 +3545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>80</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>80</v>
       </c>
@@ -3583,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>80</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>80</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>80</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>80</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>80</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>80</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>80</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>80</v>
       </c>
@@ -3748,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>80</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>80</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>80</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>80</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>80</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>80</v>
       </c>
@@ -3896,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>80</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>80</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>80</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -3990,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>80</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>80</v>
       </c>
@@ -4024,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>80</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>80</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>80</v>
       </c>
@@ -4081,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>80</v>
       </c>
@@ -4101,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>80</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>80</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>80</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>80</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>80</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -4209,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>80</v>
       </c>
@@ -4226,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>80</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>80</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>80</v>
       </c>
@@ -4277,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>80</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>80</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>80</v>
       </c>
@@ -4328,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>80</v>
       </c>
@@ -4348,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>80</v>
       </c>
@@ -4394,7 +4393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>80</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>80</v>
       </c>
@@ -4457,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>80</v>
       </c>
@@ -4477,7 +4476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>80</v>
       </c>
@@ -4494,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>80</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>80</v>
       </c>
@@ -4528,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>80</v>
       </c>
@@ -4545,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>80</v>
       </c>
@@ -4562,7 +4561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>80</v>
       </c>
@@ -4579,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>80</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>80</v>
       </c>
@@ -4613,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>80</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>80</v>
       </c>
@@ -4647,7 +4646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>80</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>80</v>
       </c>
@@ -4684,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>80</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>80</v>
       </c>
@@ -4718,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>80</v>
       </c>
@@ -4842,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>80</v>
       </c>
@@ -4859,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>80</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>80</v>
       </c>
@@ -4899,7 +4898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>80</v>
       </c>
@@ -4942,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>80</v>
       </c>
@@ -4959,7 +4958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>80</v>
       </c>
@@ -4976,7 +4975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>80</v>
       </c>
@@ -4993,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>80</v>
       </c>
@@ -5010,7 +5009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>80</v>
       </c>
@@ -5027,7 +5026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>80</v>
       </c>
@@ -5070,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>80</v>
       </c>
@@ -5087,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>80</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>80</v>
       </c>
@@ -5121,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>80</v>
       </c>
@@ -5138,7 +5137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>80</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>80</v>
       </c>
@@ -5172,7 +5171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>80</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>80</v>
       </c>
@@ -5235,7 +5234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>80</v>
       </c>
@@ -5252,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>80</v>
       </c>
@@ -5269,7 +5268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>80</v>
       </c>
@@ -5286,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>80</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>80</v>
       </c>
@@ -5320,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>80</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>80</v>
       </c>
@@ -5354,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>80</v>
       </c>
@@ -5397,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>80</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>80</v>
       </c>
@@ -5460,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>158</v>
       </c>
@@ -5480,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>158</v>
       </c>
@@ -5497,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>158</v>
       </c>
@@ -5543,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>158</v>
       </c>
@@ -5560,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>158</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>158</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>158</v>
       </c>
@@ -5640,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>158</v>
       </c>
@@ -5657,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>158</v>
       </c>
@@ -5677,7 +5676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>158</v>
       </c>
@@ -5694,7 +5693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>158</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>158</v>
       </c>
@@ -5728,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>158</v>
       </c>
@@ -5745,7 +5744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>158</v>
       </c>
@@ -5788,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>158</v>
       </c>
@@ -5805,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>158</v>
       </c>
@@ -5822,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>158</v>
       </c>
@@ -5865,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>158</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>158</v>
       </c>
@@ -5899,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>158</v>
       </c>
@@ -5917,13 +5916,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H239" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H239" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>